<commit_message>
new user programmer micro usb replacement
</commit_message>
<xml_diff>
--- a/user_programmer/BOM/user_programmer v11.xlsx
+++ b/user_programmer/BOM/user_programmer v11.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurabhdatta/PersonalProjects/clock/fusion360exports/user_programmer/BOM/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28460" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - user_programmer v11" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - user_programmer v11" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>user_programmer v11</t>
   </si>
@@ -99,7 +115,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
@@ -137,15 +153,15 @@
   <si>
     <t>USB</t>
   </si>
+  <si>
+    <t>https://lcsc.com/product-detail/USB-Connectors_Jing-Extension-of-the-Electronic-Co-920-E52A2021S10100_C10418.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -157,13 +173,13 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -304,75 +320,137 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -571,7 +649,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -590,7 +668,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -620,7 +698,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -646,7 +724,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -672,7 +750,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -698,7 +776,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -724,7 +802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -750,7 +828,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -776,7 +854,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -802,7 +880,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -828,7 +906,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -841,9 +919,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -860,7 +944,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -879,7 +963,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -905,7 +989,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -931,7 +1015,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -957,7 +1041,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -983,7 +1067,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1009,7 +1093,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1035,7 +1119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1061,7 +1145,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1087,7 +1171,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1113,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1126,9 +1210,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1142,7 +1232,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1161,7 +1251,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1191,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1217,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1243,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1269,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1295,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1321,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1347,7 +1437,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1373,7 +1463,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1399,7 +1489,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1412,219 +1502,231 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.8516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="59.0156" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37" style="1" customWidth="1"/>
+    <col min="8" max="8" width="59" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s" s="6">
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="8">
+    <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s" s="9">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="10">
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+    <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s" s="9">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s" s="10">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s" s="10">
+      <c r="E5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="F5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="8">
+    <row r="6" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s" s="9">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s" s="10">
+      <c r="C6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s" s="10">
+      <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s" s="10">
+      <c r="E6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s" s="10">
+      <c r="F6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s" s="10">
+      <c r="G6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="11"/>
+      <c r="H6" s="10"/>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
+    <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s" s="9">
+      <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s" s="10">
+      <c r="D7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s" s="10">
+      <c r="E7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s" s="10">
+      <c r="F7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="8">
+    <row r="8" spans="1:8" ht="53" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s" s="9">
+      <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s" s="10">
+      <c r="D8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E8" t="s" s="10">
+      <c r="E8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s" s="10">
+      <c r="F8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" location="" tooltip="" display="https://item.taobao.com/item.htm?spm=a1z09.2.0.0.85152e8dntbOOL&amp;id=635234737359&amp;_u=42q42hct8c07"/>
+    <hyperlink ref="G6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>